<commit_message>
changes for verify oauth security
</commit_message>
<xml_diff>
--- a/Security.xlsx
+++ b/Security.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Url</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>OAuthSecurity</t>
   </si>
 </sst>
 </file>
@@ -430,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -449,7 +452,7 @@
     <col min="1024" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,8 +471,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -483,13 +489,16 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -508,11 +517,14 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -531,8 +543,11 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -550,6 +565,9 @@
       </c>
       <c r="F6" t="s">
         <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>